<commit_message>
Added feature to send whatsapp reminders
</commit_message>
<xml_diff>
--- a/D_D_M/test.xlsx
+++ b/D_D_M/test.xlsx
@@ -337,411 +337,411 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>8:00 to 9:00</t>
+          <t>8:00 to 9:00 a.m.</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>9:00 to 10:00</t>
+          <t>9:00 to 10:00 a.m.</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>10:00 to 11:00</t>
+          <t>10:00 to 11:00 a.m.</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>11:00 to 12:00</t>
+          <t>11:00 a.m. to 12:00 p.m.</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>12:00 to 1:00</t>
+          <t>12:00 to 1:00 pm</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>2:00 to 3:00</t>
+          <t>2:00 to 3:00 p.m</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>3:00 to 4:00</t>
+          <t>3:00 to 4:00 p.m.</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>4:00 to 5:00</t>
+          <t>4:00 to 5:00 p.m.</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>5:00 to 6:00</t>
+          <t>5:00 to 6:00 p.m.</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>6:00 to 7:00</t>
+          <t>6:00 to 7:00 p.m.</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>pracheta</t>
+          <t xml:space="preserve">ASHIKKA </t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hemanth</t>
+          <t xml:space="preserve">ASHIKKA </t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Aryan Shridhar</t>
+          <t>SHRIYASHISH</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Aarush Bhat</t>
+          <t xml:space="preserve">NIYANTHA </t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Hemanth</t>
+          <t>AARUSH BHAT</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Guru </t>
+          <t>AKSHUNN TRIVEDI</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Antra </t>
+          <t>HARSHUL</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aaryan Kothari </t>
+          <t xml:space="preserve">AARYAN KOTHARI </t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ashikka </t>
+          <t xml:space="preserve">ASHIKKA </t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Poornesh Adhithya</t>
+          <t>HARSH SINGHAL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Harshul</t>
+          <t>PRACHETA</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Harshul</t>
+          <t>SHRUTI JAIN</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Guru </t>
+          <t>SOURIS ASH</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>harsh malani</t>
+          <t>HARSH SINGHAL</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>harsh singhal</t>
+          <t>HARSH MALANI</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>harsh malani</t>
+          <t xml:space="preserve">AARYAN KOTHARI </t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>harsh malani</t>
+          <t>HARSH MALANI</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Niyantha </t>
+          <t>SOURIS ASH</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Shruti jain</t>
+          <t>ISHAN D</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Agniva Basak</t>
+          <t>AGNIVA BASAK</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Soham Mittal</t>
+          <t>YASH SURYA</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Ankur</t>
+          <t>ISHAN K</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Poornesh Adhithya</t>
+          <t>POORNESH ADHITHYA</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>harsh singhal</t>
+          <t>AARUSH BHAT</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Soham Mittal</t>
+          <t>SOHAM MITTAL</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Akshunn Trivedi</t>
+          <t>HARSH MALANI</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>V Kartik</t>
+          <t>V KARTIK</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Guru </t>
+          <t>RAHUL AGARWAL</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Ishan D</t>
+          <t>SHRUTI JAIN</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Aarush Bhat</t>
+          <t>ANSH SHARMA</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>8:00 to 9:00</t>
+          <t>8:00 to 9:00 a.m.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>9:00 to 10:00</t>
+          <t>9:00 to 10:00 a.m.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>10:00 to 11:00</t>
+          <t>10:00 to 11:00 a.m.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>11:00 to 12:00</t>
+          <t>11:00 a.m. to 12:00 p.m.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>12:00 to 1:00</t>
+          <t>12:00 to 1:00 pm</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2:00 to 3:00</t>
+          <t>2:00 to 3:00 p.m</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>3:00 to 4:00</t>
+          <t>3:00 to 4:00 p.m.</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>4:00 to 5:00</t>
+          <t>4:00 to 5:00 p.m.</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>5:00 to 6:00</t>
+          <t>5:00 to 6:00 p.m.</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>6:00 to 7:00</t>
+          <t>6:00 to 7:00 p.m.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Shruti jain</t>
+          <t>SHRUTI JAIN</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Malvika </t>
+          <t>ANKUR</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>V Kartik</t>
+          <t>V KARTIK</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Niyantha </t>
+          <t>HARSH MALANI</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>V Kartik</t>
+          <t>V KARTIK</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>V Kartik</t>
+          <t>V KARTIK</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Ishan D</t>
+          <t>ISHAN D</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Ishan D</t>
+          <t>ISHAN D</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Ankur</t>
+          <t>ANKUR</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Khyati</t>
+          <t>AARUSH BHAT</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>khushboo</t>
+          <t>KHUSHBOO</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Shruti jain</t>
+          <t>HEMANTH</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>khushboo</t>
+          <t>KHUSHBOO</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Shubham</t>
+          <t>SHUBHAM</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Aarush Bhat</t>
+          <t>HEMANTH</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Ishan D</t>
+          <t>ISHAN D</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Harshul</t>
+          <t xml:space="preserve">ANTRA </t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>yash surya</t>
+          <t xml:space="preserve">NIYANTHA </t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Agniva Basak</t>
+          <t>AGNIVA BASAK</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Antra </t>
+          <t>KHYATI</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>yash surya</t>
+          <t>SHRIYASHISH</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>khushboo</t>
+          <t xml:space="preserve">MALVIKA </t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Shriyashish</t>
+          <t>GURU AATHAVAN</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Niyantha </t>
+          <t xml:space="preserve">NIYANTHA </t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Antra </t>
+          <t xml:space="preserve">ANTRA </t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aaryan Kothari </t>
+          <t xml:space="preserve">AARYAN KOTHARI </t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Souish Ash</t>
+          <t>YASH SURYA</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Ishan K</t>
+          <t>ISHAN K</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>harsh malani</t>
+          <t xml:space="preserve">ANTRA </t>
         </is>
       </c>
     </row>
@@ -767,309 +767,292 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>8:00 to 9:00</t>
+          <t>8:00 to 9:00 a.m.</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>9:00 to 10:00</t>
+          <t>9:00 to 10:00 a.m.</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>10:00 to 11:00</t>
+          <t>10:00 to 11:00 a.m.</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>11:00 to 12:00</t>
+          <t>11:00 a.m. to 12:00 p.m.</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>12:00 to 1:00</t>
+          <t>12:00 to 1:00 pm</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>2:00 to 3:00</t>
+          <t>2:00 to 3:00 p.m</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>3:00 to 4:00</t>
+          <t>3:00 to 4:00 p.m.</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>4:00 to 5:00</t>
+          <t>4:00 to 5:00 p.m.</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>5:00 to 6:00</t>
+          <t>5:00 to 6:00 p.m.</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>6:00 to 7:00</t>
+          <t>6:00 to 7:00 p.m.</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ansh Sharma</t>
+          <t>HARSH SINGHAL</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Aryan Shridhar</t>
+          <t>ANSH SHARMA</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Akshunn Trivedi </t>
+          <t>SHAKTHI DHAR</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>SRISHTI</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Shakthi Dhar</t>
+          <t>SOHAM MITTAL</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>harsh</t>
+          <t>KHUSHBOO</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Ashikka</t>
+          <t>V KARTIK</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Harshul</t>
+          <t>DSP</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Antra</t>
+          <t>HARSHUL</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Rahul Agarwal</t>
+          <t>SOURIS ASH</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>harsh singhal</t>
+          <t>KHUSHBOO</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>harsh</t>
+          <t>HARSHUL</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Srishti</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>r</t>
+          <t xml:space="preserve">AKSHUNN TRIVEDI </t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>pracheta</t>
+          <t>ANSH SHARMA</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>V Kartik</t>
+          <t>SHRIYASHISH</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Poornesh Adhithya</t>
+          <t>ANSH SHARMA</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Khyati</t>
+          <t>SHRUTI JAIN</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Harshul</t>
+          <t>ANTRA</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>yash surya</t>
+          <t>HARSHUL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Shriyashish</t>
+          <t>SOHAM MITTAL</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Aarush Bhat</t>
+          <t>KHUSHBOO</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve">divya </t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>i</t>
+          <t xml:space="preserve">DIVYA </t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Akshunn Trivedi </t>
+          <t>PRACHETA</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Shriyashish</t>
+          <t>V KARTIK</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Agniva Basak</t>
+          <t>HEMANTH</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Antra</t>
+          <t>ANTRA</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Khyati</t>
+          <t>KHYATI</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Harshul</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>s</t>
+          <t>ANSH SHARMA</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>8:00 to 9:00</t>
+          <t>8:00 to 9:00 a.m.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>9:00 to 10:00</t>
+          <t>9:00 to 10:00 a.m.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>10:00 to 11:00</t>
+          <t>10:00 to 11:00 a.m.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>h</t>
+          <t>11:00 a.m. to 12:00 p.m.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>12:00 to 1:00</t>
+          <t>12:00 to 1:00 pm</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2:00 to 3:00</t>
+          <t>2:00 to 3:00 p.m</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>3:00 to 4:00</t>
+          <t>3:00 to 4:00 p.m.</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>4:00 to 5:00</t>
+          <t>4:00 to 5:00 p.m.</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>5:00 to 6:00</t>
+          <t>5:00 to 6:00 p.m.</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>6:00 to 7:00</t>
+          <t>6:00 to 7:00 p.m.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>khushboo</t>
+          <t>SHRIYASHISH</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>V Kartik</t>
+          <t>V KARTIK</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Shakthi Dhar</t>
+          <t>MALVIKA</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Khyati</t>
+          <t>KHYATI</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Khyati</t>
+          <t>KHYATI</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>khushboo</t>
+          <t>HARSH MALANI</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>V Kartik</t>
+          <t>AARUSH BHAT</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Ankur</t>
+          <t>KHYATI</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -1079,96 +1062,96 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Khyati</t>
+          <t>KHYATI</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Soham Mittal</t>
+          <t>ANSH SHARMA</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Ankur</t>
+          <t>AARUSH BHAT</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Malvika</t>
+          <t>HARSHUL</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Srishti</t>
+          <t>SRISHTI</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Antra</t>
+          <t>ANTRA</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Ishan D</t>
+          <t>ISHAN D</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Aarush Bhat</t>
+          <t>AGNIVA BASAK</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Shruti Jain</t>
+          <t>ANKUR</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Antra</t>
+          <t>ANTRA</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Rohan Arora</t>
+          <t>ROHAN ARORA</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Shakthi Dhar</t>
+          <t>ANKUR</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Harshul</t>
+          <t>SRISHTI</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Ashikka</t>
+          <t>ASHIKKA</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Srishti</t>
+          <t>SHAKTHI DHAR</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>harsh</t>
+          <t>HARSH MALANI</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>DSP</t>
+          <t>HARSHUL</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Malvika</t>
+          <t>MALVIKA</t>
         </is>
       </c>
     </row>
@@ -1183,7 +1166,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1194,94 +1177,94 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>8:00 to 9:00</t>
+          <t>8:00 to 9:00 a.m.</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>9:00 to 10:00</t>
+          <t>9:00 to 10:00 a.m.</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>10:00 to 11:00</t>
+          <t>10:00 to 11:00 a.m.</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>11:00 to 12:00</t>
+          <t>11:00 a.m. to 12:00 p.m.</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>12:00 to 1:00</t>
+          <t>12:00 to 1:00 pm</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>2:00 to 3:00</t>
+          <t>2:00 to 3:00 p.m</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>3:00 to 4:00</t>
+          <t>3:00 to 4:00 p.m.</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>4:00 to 5:00</t>
+          <t>4:00 to 5:00 p.m.</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>5:00 to 6:00</t>
+          <t>5:00 to 6:00 p.m.</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>6:00 to 7:00</t>
+          <t>6:00 to 7:00 p.m.</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>POORNESH ADHITHYA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>p</t>
+          <t>PRACHETA</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Ankur</t>
+          <t>AASTHA SINGH</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Ansh Sharma</t>
+          <t>KHYATI</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Shubham</t>
+          <t>ADI</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Harshul</t>
+          <t>KHYATI</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>adi</t>
+          <t>ADI</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Rahul Agarwal</t>
+          <t>RAHUL AGARWAL</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -1291,212 +1274,180 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Poornesh Adhithya</t>
+          <t>SHRUTI JAIN</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>r</t>
-        </is>
-      </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Ashikka</t>
+          <t>HEMANTH</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>V Kartik</t>
+          <t>ANTRA</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>yash surya</t>
+          <t>SOURIS ASH</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Ashikka</t>
+          <t>ANTRA</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Harshul</t>
+          <t>SOHAM MITTAL</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>harsh</t>
+          <t>HARSH MALANI</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>yash surya</t>
+          <t>GURU AATHAVAN</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Ashikka</t>
+          <t>ANSH SHARMA</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Hemanth</t>
+          <t>MALVIKA</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Hemanth</t>
+          <t>ISHAN D</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Ishan K</t>
+          <t>MALVIKA</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Rahul Agarwal</t>
+          <t xml:space="preserve">AARYAN KOTHARI </t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Guru Aathavan</t>
+          <t>ANTRA</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>harsh</t>
+          <t>HARSH SINGHAL</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Guru Aathavan</t>
+          <t>AKSHUNN TRIVEDI</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Shriyashish </t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>r</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>c</t>
+          <t>ARYAN SHRIDHAR</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>n</t>
+          <t>8:00 to 9:00 a.m.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>h</t>
+          <t>9:00 to 10:00 a.m.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>10:00 to 11:00</t>
+          <t>10:00 to 11:00 a.m.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>11:00 to 12:00</t>
+          <t>11:00 a.m. to 12:00 p.m.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>12:00 to 1:00</t>
+          <t>12:00 to 1:00 pm</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2:00 to 3:00</t>
+          <t>2:00 to 3:00 p.m</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>3:00 to 4:00</t>
+          <t>3:00 to 4:00 p.m.</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>4:00 to 5:00</t>
+          <t>4:00 to 5:00 p.m.</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>5:00 to 6:00</t>
+          <t>5:00 to 6:00 p.m.</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>6:00 to 7:00</t>
+          <t>6:00 to 7:00 p.m.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>pracheta</t>
+          <t>PRACHETA</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Shubham</t>
+          <t>SHUBHAM</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Malvika</t>
+          <t>ANKUR</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Khyati</t>
+          <t>V KARTIK</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>V Kartik</t>
+          <t>V KARTIK</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Khyati</t>
+          <t>NIYANTHA</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Khyati</t>
+          <t>KHYATI</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -1506,164 +1457,96 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Akshunn Trivedi</t>
+          <t>YASH SURYA</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Shruti Jain</t>
+          <t>MALVIKA</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Poornesh Adhithya</t>
+          <t>POORNESH ADHITHYA</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>pracheta</t>
+          <t>PRACHETA</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Srishti</t>
+          <t>SRISHTI</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Aarush bhat</t>
+          <t>AARUSH BHAT</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Khyati</t>
+          <t>KHYATI</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Antra</t>
+          <t>KHUSHBOO</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Shakthi Dhar</t>
+          <t>SHAKTHI DHAR</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Aastha Singh</t>
+          <t>AASTHA SINGH</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Malvika</t>
+          <t>YASH SURYA</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>h</t>
-        </is>
-      </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>divya</t>
+          <t>DIVYA</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Aastha Singh</t>
+          <t>ASHIKKA</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Ankur</t>
+          <t>ANKUR</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Aarush bhat</t>
+          <t>AARUSH BHAT</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Niyantha</t>
+          <t xml:space="preserve">SHRIYASHISH </t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Antra</t>
+          <t>NIYANTHA</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>yash surya</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>d</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>h</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>i</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>t</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>h</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>y</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>a</t>
+          <t>KHUSHBOO</t>
         </is>
       </c>
     </row>
@@ -1689,401 +1572,401 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>8:00 to 9:00</t>
+          <t>8:00 to 9:00 a.m.</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>9:00 to 10:00</t>
+          <t>9:00 to 10:00 a.m.</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>10:00 to 11:00</t>
+          <t>10:00 to 11:00 a.m.</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>11:00 to 12:00</t>
+          <t>11:00 a.m. to 12:00 p.m.</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>12:00 to 1:00</t>
+          <t>12:00 to 1:00 pm</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>2:00 to 3:00</t>
+          <t>2:00 to 3:00 p.m</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>3:00 to 4:00</t>
+          <t>3:00 to 4:00 p.m.</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>4:00 to 5:00</t>
+          <t>4:00 to 5:00 p.m.</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>5:00 to 6:00</t>
+          <t>5:00 to 6:00 p.m.</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>6:00 to 7:00</t>
+          <t>6:00 to 7:00 p.m.</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>yash surya</t>
+          <t>V KARTIK</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ansh Sharma</t>
+          <t>ASHIKKA</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>harsh singhal</t>
+          <t>SRISHTI</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Souris Ash</t>
+          <t>HARSHUL</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Niyantha</t>
+          <t>V KARTIK</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aaryan kothari </t>
+          <t>GURU AATHAVAN</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>harsh singhal</t>
+          <t>SHAKTHI DHAR</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Souris Ash</t>
+          <t>HARSHUL</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Aarush Bhat</t>
+          <t>ANKUR</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>harsh</t>
+          <t>POORNESH ADHITHYA</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>V Kartik</t>
+          <t xml:space="preserve">AARYAN KOTHARI </t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>yash surya</t>
+          <t>SHUBHAM</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>harsh</t>
+          <t>ARYAN SHRIDHAR</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>shriyashish</t>
+          <t>SHRIYASHISH</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>V Kartik</t>
+          <t>AGNIVA BASAK</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Shubham</t>
+          <t>HARSH MALANI</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>V Kartik</t>
+          <t>SHUBHAM</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Agniva Basak</t>
+          <t>ASHIKKA</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Antra</t>
+          <t>ANTRA</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>V Kartik</t>
+          <t>YASH SURYA</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aaryan kothari </t>
+          <t>MALVIKA</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Ashikka</t>
+          <t>GURU AATHAVAN</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Aarush Bhat</t>
+          <t>KHUSHBOO</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Guru Aathavan</t>
+          <t>GURU AATHAVAN</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Agniva Basak</t>
+          <t>GURU AATHAVAN</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>pracheta</t>
+          <t>AASTHA SINGH</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Aarush Bhat</t>
+          <t>NIYANTHA</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Ashikka</t>
+          <t>SOURIS ASH</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Ankur</t>
+          <t>AARUSH BHAT</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>harsh singhal</t>
+          <t>HARSH MALANI</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>8:00 to 9:00</t>
+          <t>8:00 to 9:00 a.m.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>9:00 to 10:00</t>
+          <t>9:00 to 10:00 a.m.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>10:00 to 11:00</t>
+          <t>10:00 to 11:00 a.m.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>11:00 to 12:00</t>
+          <t>11:00 a.m. to 12:00 p.m.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>12:00 to 1:00</t>
+          <t>12:00 to 1:00 pm</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2:00 to 3:00</t>
+          <t>2:00 to 3:00 p.m</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>3:00 to 4:00</t>
+          <t>3:00 to 4:00 p.m.</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>4:00 to 5:00</t>
+          <t>4:00 to 5:00 p.m.</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>5:00 to 6:00</t>
+          <t>5:00 to 6:00 p.m.</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>6:00 to 7:00</t>
+          <t>6:00 to 7:00 p.m.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Malvika</t>
+          <t>YASH SURYA</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>harsh singhal</t>
+          <t>YASH SURYA</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>V Kartik</t>
+          <t>V KARTIK</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>khushboo</t>
+          <t>KHUSHBOO</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Hemanth</t>
+          <t>HEMANTH</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>V Kartik</t>
+          <t>V KARTIK</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Shakthi Dhar</t>
+          <t>V KARTIK</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Khyati</t>
+          <t>KHYATI</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Shruti Jain</t>
+          <t>SHRUTI JAIN</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Aarush Bhat</t>
+          <t>V KARTIK</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Poornesh Adhithya</t>
+          <t>POORNESH ADHITHYA</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Guru Aathavan</t>
+          <t>HARSH SINGHAL</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Ankur</t>
+          <t>AARUSH BHAT</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Harshul</t>
+          <t>SOURIS ASH</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Antra</t>
+          <t>ANTRA</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Aarush Bhat</t>
+          <t>AARUSH BHAT</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Niyantha</t>
+          <t>AARUSH BHAT</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Aarush Bhat</t>
+          <t>AARUSH BHAT</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Ankur</t>
+          <t>AARUSH BHAT</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="inlineStr">
         <is>
-          <t>Shubham</t>
+          <t>ANSH SHARMA</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Shakthi Dhar</t>
+          <t>ANKUR</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Soham Mittal</t>
+          <t>SOHAM MITTAL</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>khushboo</t>
+          <t>NIYANTHA</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Shakthi Dhar</t>
+          <t>SHAKTHI DHAR</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>harsh</t>
+          <t>HARSH MALANI</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Antra</t>
+          <t>ANTRA</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Antra</t>
+          <t>ANKUR</t>
         </is>
       </c>
     </row>
@@ -2109,416 +1992,416 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>8:00 to 9:00</t>
+          <t>8:00 to 9:00 a.m.</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>9:00 to 10:00</t>
+          <t>9:00 to 10:00 a.m.</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>10:00 to 11:00</t>
+          <t>10:00 to 11:00 a.m.</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>11:00 to 12:00</t>
+          <t>11:00 a.m. to 12:00 p.m.</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>12:00 to 1:00</t>
+          <t>12:00 to 1:00 pm</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>2:00 to 3:00</t>
+          <t>2:00 to 3:00 p.m</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>3:00 to 4:00</t>
+          <t>3:00 to 4:00 p.m.</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>4:00 to 5:00</t>
+          <t>4:00 to 5:00 p.m.</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>5:00 to 6:00</t>
+          <t>5:00 to 6:00 p.m.</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>6:00 to 7:00</t>
+          <t>6:00 to 7:00 p.m.</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ansh Sharma</t>
+          <t>PRACHETA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Aastha Singh</t>
+          <t>SRISHTI</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Ishan K</t>
+          <t>YASH SURYA</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Agniva Basak</t>
+          <t>AGNIVA BASAK</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>V Kartik</t>
+          <t xml:space="preserve">AARYAN KOTHARI </t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aaryan kothari </t>
+          <t>AARUSH BHAT</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Niyantha </t>
+          <t>HARSH MALANI</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Guru Aathavan</t>
+          <t>V KARTIK</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Aarush Bhat</t>
+          <t>DSP</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Rahul Agarwal</t>
+          <t>YASH SURYA</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Poornesh Adhithya</t>
+          <t>GURU AATHAVAN</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Srishti</t>
+          <t>SHRUTI JAIN</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Shubham</t>
+          <t>ASHIKKA</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Hemanth</t>
+          <t>ASHIKKA</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Aryan Shridhar</t>
+          <t>POORNESH ADHITHYA</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>V Kartik</t>
+          <t>V KARTIK</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Harshul</t>
+          <t>ANTRA</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
+          <t>HARSH MALANI</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>V KARTIK</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
           <t>DSP</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Shakthi Dhar</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Archisman Hota</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Shruti Jain</t>
+          <t>DSP</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>pracheta</t>
+          <t>AASTHA SINGH</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Guru Aathavan</t>
+          <t>GURU AATHAVAN</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Ashikka</t>
+          <t>SRISHTI</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Archisman Hota</t>
+          <t>ADI</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Rahul Agarwal</t>
+          <t>ANTRA</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Antra</t>
+          <t>V KARTIK</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Ansh Sharma</t>
+          <t>ADI</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Niyantha </t>
+          <t>ANSH SHARMA</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Shruti Jain</t>
+          <t>AKSHUNN TRIVEDI</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>8:00 to 9:00</t>
+          <t>8:00 to 9:00 a.m.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>9:00 to 10:00</t>
+          <t>9:00 to 10:00 a.m.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>10:00 to 11:00</t>
+          <t>10:00 to 11:00 a.m.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>11:00 to 12:00</t>
+          <t>11:00 a.m. to 12:00 p.m.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>12:00 to 1:00</t>
+          <t>12:00 to 1:00 pm</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2:00 to 3:00</t>
+          <t>2:00 to 3:00 p.m</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>3:00 to 4:00</t>
+          <t>3:00 to 4:00 p.m.</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>4:00 to 5:00</t>
+          <t>4:00 to 5:00 p.m.</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>5:00 to 6:00</t>
+          <t>5:00 to 6:00 p.m.</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>6:00 to 7:00</t>
+          <t>6:00 to 7:00 p.m.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Shakthi Dhar</t>
+          <t>SHAKTHI DHAR</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Shruti Jain</t>
+          <t>GURU AATHAVAN</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Hemanth</t>
+          <t>HEMANTH</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Srishti</t>
+          <t>HEMANTH</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>yash surya</t>
+          <t>V KARTIK</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Khyati</t>
+          <t>KHYATI</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>V Kartik</t>
+          <t>AARUSH BHAT</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>V Kartik</t>
+          <t>AARUSH BHAT</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>V Kartik</t>
+          <t>AARUSH BHAT</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>V Kartik</t>
+          <t>V KARTIK</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Akshunn Trivedi</t>
+          <t>SHRUTI JAIN</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Guru Aathavan</t>
+          <t>PRACHETA</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Agniva Basak</t>
+          <t>AGNIVA BASAK</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Poornesh Adhithya</t>
+          <t>POORNESH ADHITHYA</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Souris Ash</t>
+          <t>YASH SURYA</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Aarush Bhat</t>
+          <t>HARSH MALANI</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Aarush Bhat</t>
+          <t xml:space="preserve">NIYANTHA </t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Aarush Bhat</t>
+          <t>SHAKTHI DHAR</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Rahul Agarwal</t>
+          <t>SHAKTHI DHAR</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Khyati</t>
+          <t>KHYATI</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Guru Aathavan</t>
+          <t>AKSHUNN TRIVEDI</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Ishan K</t>
+          <t>ISHAN K</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Malvika</t>
+          <t>MALVIKA</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Rohan Arora</t>
+          <t>ROHAN ARORA</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Srishti</t>
+          <t>SOURIS ASH</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Antra</t>
+          <t xml:space="preserve">NIYANTHA </t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>harsh</t>
+          <t>HARSH SINGHAL</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Shakthi Dhar</t>
+          <t xml:space="preserve">NIYANTHA </t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Ansh Sharma</t>
+          <t xml:space="preserve">NIYANTHA </t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Aarush Bhat</t>
+          <t>AARUSH BHAT</t>
         </is>
       </c>
     </row>

</xml_diff>